<commit_message>
add tasking for core domain
</commit_message>
<xml_diff>
--- a/credit card/credit card.xlsx
+++ b/credit card/credit card.xlsx
@@ -12,6 +12,59 @@
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>core tasking</t>
+  </si>
+  <si>
+    <t>credit card charges generation</t>
+  </si>
+  <si>
+    <t>generate credit card charge</t>
+  </si>
+  <si>
+    <t>eg:customer request one consume request and then generate a charge</t>
+  </si>
+  <si>
+    <t>generate payable without periods</t>
+  </si>
+  <si>
+    <t>after customer's credit card charge, he will receive a payable in one period</t>
+  </si>
+  <si>
+    <t>Credit cards charges payment</t>
+  </si>
+  <si>
+    <t>charge for non cash deal</t>
+  </si>
+  <si>
+    <t>eg:during the payment, bank money decrease, shop owner money increase</t>
+  </si>
+  <si>
+    <t>charge for cash deal</t>
+  </si>
+  <si>
+    <t>eg:after the payment, customer receive money, bank money decrease</t>
+  </si>
+  <si>
+    <t>payable bill payment</t>
+  </si>
+  <si>
+    <t>pay for a payable bill with only one payable</t>
+  </si>
+  <si>
+    <t>eg:customer pay a payable bill with one payable</t>
+  </si>
+  <si>
+    <t>pay for a payable bill with more than one payable</t>
+  </si>
+  <si>
+    <t>eg:customer pay a payable bill with two payables</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -110,22 +163,105 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.0663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4489795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.0663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.8418367346939"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>